<commit_message>
Revert "Merge branch 'main' of https://github.com/HKiet-dev/G4U"
This reverts commit 842240d5c4b4e066928ac08bbb2bf0b7d3e46005, reversing
changes made to 6da871fc41065db8084bd37572eb2ee6f627569d.
</commit_message>
<xml_diff>
--- a/Report/Requirement (1).xlsx
+++ b/Report/Requirement (1).xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28105"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28014"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FPT Polytechnic\Graduation\G4U\Report\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FPT Polytechnic\Graduation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B79ECDD3-61AC-4C76-B310-E6F2B047903F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55799C48-460A-454D-82DA-2AF184663F1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{66551FA1-06BE-4D31-8093-516AC48B2C2B}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="99">
   <si>
     <t>Requirements Description</t>
   </si>
@@ -195,6 +195,12 @@
     <t>Thống kê (in pdf, excel)</t>
   </si>
   <si>
+    <t>Báo cáo game</t>
+  </si>
+  <si>
+    <t>Thanh toán (momo, vnpay, COD)</t>
+  </si>
+  <si>
     <t>Role</t>
   </si>
   <si>
@@ -237,6 +243,9 @@
     <t>Kiệt</t>
   </si>
   <si>
+    <t>Đang tìm hiểu...</t>
+  </si>
+  <si>
     <t>Thống kế số lượng, số lượng chơi game từng sp,…. Có in file excel, pdf</t>
   </si>
   <si>
@@ -258,6 +267,9 @@
     <t>Đăng nhập đăng kí tài khoản bình thường</t>
   </si>
   <si>
+    <t>Báo cáo game không phù hợp, game lỗi</t>
+  </si>
+  <si>
     <t>Lọc theo thể loại, theo tuổi, theo giá</t>
   </si>
   <si>
@@ -279,9 +291,15 @@
     <t>down bằng link của ggdrive với terrabox</t>
   </si>
   <si>
+    <t>lấy c#6 ra mà làm</t>
+  </si>
+  <si>
     <t>Xem, chỉnh sửa hồ sơ, đổi mk</t>
   </si>
   <si>
+    <t>tương tự</t>
+  </si>
+  <si>
     <t>Hiện thời gian, trạng thái, sản phẩm đã mua</t>
   </si>
   <si>
@@ -322,51 +340,6 @@
   </si>
   <si>
     <t>Tần, Hưng, Nhân</t>
-  </si>
-  <si>
-    <t>Đưa hình ảnh lên AI kiểm tra</t>
-  </si>
-  <si>
-    <t>Dùng Google Adsense</t>
-  </si>
-  <si>
-    <t>Thanh toán (momo, vpn)</t>
-  </si>
-  <si>
-    <t>Thanh toán qua các hình thức online banking</t>
-  </si>
-  <si>
-    <t>Chỉnh sửa thông tin cá nhân: tên hiển thị, avatar, số điện thoại</t>
-  </si>
-  <si>
-    <t>Thêm sản phẩm yêu thích vào wishlist</t>
-  </si>
-  <si>
-    <t>Thêm xóa sửa các sản phẩm yêu thích</t>
-  </si>
-  <si>
-    <t>Tố cáo game</t>
-  </si>
-  <si>
-    <t>Tố cáo game không phù hợp, game lỗi</t>
-  </si>
-  <si>
-    <t>Admin-1</t>
-  </si>
-  <si>
-    <t>Admin-3</t>
-  </si>
-  <si>
-    <t>Admin-5</t>
-  </si>
-  <si>
-    <t>Admin-2</t>
-  </si>
-  <si>
-    <t>Admin-4</t>
-  </si>
-  <si>
-    <t>Admin-6</t>
   </si>
 </sst>
 </file>
@@ -424,7 +397,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -610,7 +585,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -665,7 +640,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -699,18 +673,29 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1093,7 +1078,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:pivotSource>
-    <c:name>[Requirement (1).xlsx]Status!PivotTable5</c:name>
+    <c:name>[Requirement.xlsx]Status!PivotTable5</c:name>
     <c:fmtId val="0"/>
   </c:pivotSource>
   <c:chart>
@@ -2775,7 +2760,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D670A074-11C2-4534-81DA-C65028B9F80D}" name="Table2" displayName="Table2" ref="A7:T33" totalsRowShown="0" headerRowDxfId="32" dataDxfId="31">
   <autoFilter ref="A7:T33" xr:uid="{40ACC06F-DF0F-4565-AB81-61F9F81BAAF1}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A8:T33">
-    <sortCondition ref="A7:A33"/>
+    <sortCondition ref="T7:T33"/>
   </sortState>
   <tableColumns count="20">
     <tableColumn id="1" xr3:uid="{64031A45-824B-4700-8A01-8F0F87C05385}" name="Req. ID" dataDxfId="30"/>
@@ -3102,8 +3087,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7551B106-1BC4-4794-8DF3-1BDFDAFF6E5D}">
   <dimension ref="A1:V321"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3145,11 +3130,11 @@
       <c r="P1" s="4"/>
       <c r="Q1" s="5"/>
       <c r="R1" s="4"/>
-      <c r="T1" s="21" t="s">
+      <c r="T1" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="U1" s="21"/>
-      <c r="V1" s="21"/>
+      <c r="U1" s="20"/>
+      <c r="V1" s="20"/>
     </row>
     <row r="2" spans="1:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
@@ -3170,11 +3155,11 @@
       <c r="P2" s="4"/>
       <c r="Q2" s="5"/>
       <c r="R2" s="4"/>
-      <c r="T2" s="22" t="s">
+      <c r="T2" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="U2" s="22"/>
-      <c r="V2" s="22"/>
+      <c r="U2" s="21"/>
+      <c r="V2" s="21"/>
     </row>
     <row r="3" spans="1:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
@@ -3183,57 +3168,57 @@
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
-      <c r="G3" s="31" t="s">
+      <c r="G3" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="H3" s="31"/>
-      <c r="I3" s="31"/>
-      <c r="J3" s="31"/>
-      <c r="K3" s="31"/>
-      <c r="L3" s="31"/>
-      <c r="M3" s="31"/>
-      <c r="N3" s="31"/>
-      <c r="O3" s="31"/>
+      <c r="H3" s="30"/>
+      <c r="I3" s="30"/>
+      <c r="J3" s="30"/>
+      <c r="K3" s="30"/>
+      <c r="L3" s="30"/>
+      <c r="M3" s="30"/>
+      <c r="N3" s="30"/>
+      <c r="O3" s="30"/>
       <c r="P3" s="4"/>
       <c r="Q3" s="5"/>
       <c r="R3" s="4"/>
-      <c r="T3" s="22" t="s">
+      <c r="T3" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="U3" s="22"/>
-      <c r="V3" s="22"/>
+      <c r="U3" s="21"/>
+      <c r="V3" s="21"/>
     </row>
     <row r="4" spans="1:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="28" t="s">
+      <c r="A4" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="28"/>
-      <c r="C4" s="29" t="s">
+      <c r="B4" s="27"/>
+      <c r="C4" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="D4" s="30"/>
+      <c r="D4" s="29"/>
       <c r="E4" s="19"/>
       <c r="F4" s="4"/>
-      <c r="G4" s="31"/>
-      <c r="H4" s="31"/>
-      <c r="I4" s="31"/>
-      <c r="J4" s="31"/>
-      <c r="K4" s="31"/>
-      <c r="L4" s="31"/>
-      <c r="M4" s="31"/>
-      <c r="N4" s="31"/>
-      <c r="O4" s="31"/>
+      <c r="G4" s="30"/>
+      <c r="H4" s="30"/>
+      <c r="I4" s="30"/>
+      <c r="J4" s="30"/>
+      <c r="K4" s="30"/>
+      <c r="L4" s="30"/>
+      <c r="M4" s="30"/>
+      <c r="N4" s="30"/>
+      <c r="O4" s="30"/>
       <c r="P4" s="4"/>
       <c r="Q4" s="5"/>
       <c r="R4" s="4"/>
     </row>
     <row r="5" spans="1:22" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="27" t="s">
+      <c r="A5" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="27"/>
-      <c r="C5" s="29"/>
-      <c r="D5" s="30"/>
+      <c r="B5" s="26"/>
+      <c r="C5" s="28"/>
+      <c r="D5" s="29"/>
       <c r="E5" s="19"/>
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
@@ -3250,29 +3235,29 @@
       <c r="R5" s="4"/>
     </row>
     <row r="6" spans="1:22" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="23" t="s">
+      <c r="A6" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="24"/>
-      <c r="C6" s="25"/>
-      <c r="D6" s="25"/>
-      <c r="E6" s="25"/>
-      <c r="F6" s="26"/>
-      <c r="G6" s="23" t="s">
+      <c r="B6" s="23"/>
+      <c r="C6" s="24"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="25"/>
+      <c r="G6" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="H6" s="24"/>
-      <c r="I6" s="24"/>
-      <c r="J6" s="24"/>
-      <c r="K6" s="24"/>
-      <c r="L6" s="24"/>
-      <c r="M6" s="24"/>
-      <c r="N6" s="26"/>
-      <c r="O6" s="23" t="s">
+      <c r="H6" s="23"/>
+      <c r="I6" s="23"/>
+      <c r="J6" s="23"/>
+      <c r="K6" s="23"/>
+      <c r="L6" s="23"/>
+      <c r="M6" s="23"/>
+      <c r="N6" s="25"/>
+      <c r="O6" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="P6" s="24"/>
-      <c r="Q6" s="26"/>
+      <c r="P6" s="23"/>
+      <c r="Q6" s="25"/>
       <c r="R6" s="3"/>
     </row>
     <row r="7" spans="1:22" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
@@ -3334,18 +3319,16 @@
         <v>12</v>
       </c>
       <c r="T7" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A8" s="9">
-        <v>1</v>
-      </c>
-      <c r="B8" s="20" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="9"/>
+      <c r="B8" s="34" t="s">
+        <v>58</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>59</v>
-      </c>
-      <c r="C8" s="36" t="s">
-        <v>70</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="10">
@@ -3369,23 +3352,21 @@
       <c r="S8" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="T8" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A9" s="12">
-        <v>2</v>
-      </c>
-      <c r="B9" t="s">
-        <v>39</v>
+      <c r="T8" s="31" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="12"/>
+      <c r="B9" s="35" t="s">
+        <v>60</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="D9" s="1"/>
+        <v>62</v>
+      </c>
+      <c r="D9" s="31"/>
       <c r="E9" s="10">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>29</v>
@@ -3404,19 +3385,17 @@
       <c r="S9" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="T9" s="1" t="s">
-        <v>51</v>
+      <c r="T9" s="31" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A10" s="9">
-        <v>3</v>
-      </c>
-      <c r="B10" t="s">
-        <v>37</v>
+      <c r="A10" s="9"/>
+      <c r="B10" s="35" t="s">
+        <v>46</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1">
@@ -3439,23 +3418,21 @@
       <c r="S10" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="T10" s="1" t="s">
+      <c r="T10" s="31" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A11" s="12">
-        <v>4</v>
-      </c>
-      <c r="B11" t="s">
-        <v>35</v>
+      <c r="A11" s="12"/>
+      <c r="B11" s="35" t="s">
+        <v>44</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>29</v>
@@ -3474,23 +3451,21 @@
       <c r="S11" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="T11" s="1" t="s">
-        <v>51</v>
+      <c r="T11" s="31" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A12" s="9">
-        <v>5</v>
-      </c>
-      <c r="B12" t="s">
-        <v>78</v>
-      </c>
-      <c r="C12" s="10" t="s">
-        <v>97</v>
+      <c r="A12" s="9"/>
+      <c r="B12" s="35" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" s="38" t="s">
+        <v>66</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>29</v>
@@ -3509,59 +3484,58 @@
       <c r="S12" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="T12" s="1" t="s">
-        <v>52</v>
+      <c r="T12" s="31" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A13" s="12">
-        <v>6</v>
-      </c>
+      <c r="A13" s="12"/>
       <c r="B13" s="35" t="s">
-        <v>33</v>
-      </c>
-      <c r="C13" s="34" t="s">
-        <v>68</v>
+        <v>47</v>
+      </c>
+      <c r="C13" s="38" t="s">
+        <v>66</v>
       </c>
       <c r="D13" s="1"/>
-      <c r="E13" s="36">
-        <v>1</v>
-      </c>
-      <c r="F13" s="36" t="s">
+      <c r="E13" s="1">
+        <v>4</v>
+      </c>
+      <c r="F13" s="1" t="s">
         <v>29</v>
       </c>
       <c r="G13" s="13"/>
       <c r="H13" s="12"/>
-      <c r="I13" s="36"/>
-      <c r="J13" s="36"/>
-      <c r="K13" s="36"/>
-      <c r="L13" s="36"/>
-      <c r="M13" s="36"/>
-      <c r="N13" s="36"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
       <c r="O13" s="13"/>
       <c r="P13" s="12"/>
-      <c r="Q13" s="36"/>
       <c r="R13" s="13"/>
       <c r="S13" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="T13" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A14" s="9">
-        <v>7</v>
-      </c>
-      <c r="B14" t="s">
-        <v>34</v>
-      </c>
-      <c r="C14" s="36" t="s">
-        <v>72</v>
+      <c r="T13" s="31" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="9"/>
+      <c r="B14" s="35" t="s">
+        <v>49</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
+      <c r="E14" s="1">
+        <v>5</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="G14" s="13"/>
       <c r="H14" s="12"/>
       <c r="I14" s="1"/>
@@ -3573,22 +3547,24 @@
       <c r="O14" s="13"/>
       <c r="P14" s="12"/>
       <c r="R14" s="13"/>
-      <c r="S14" s="17"/>
-      <c r="T14" s="1"/>
-    </row>
-    <row r="15" spans="1:22" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="12">
-        <v>8</v>
-      </c>
-      <c r="B15" t="s">
-        <v>73</v>
+      <c r="S14" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="T14" s="31" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A15" s="12"/>
+      <c r="B15" s="35" t="s">
+        <v>45</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="D15" s="1"/>
-      <c r="E15" s="1">
-        <v>3</v>
+      <c r="E15" s="32">
+        <v>10</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>29</v>
@@ -3607,23 +3583,21 @@
       <c r="S15" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="T15" s="1" t="s">
-        <v>54</v>
+      <c r="T15" s="31" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A16" s="12">
-        <v>9</v>
-      </c>
-      <c r="B16" t="s">
-        <v>36</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>71</v>
+      <c r="A16" s="12"/>
+      <c r="B16" s="35" t="s">
+        <v>50</v>
+      </c>
+      <c r="C16" s="32" t="s">
+        <v>74</v>
       </c>
       <c r="D16" s="1"/>
       <c r="E16" s="1">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>29</v>
@@ -3642,19 +3616,17 @@
       <c r="S16" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="T16" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A17" s="9">
-        <v>10</v>
-      </c>
-      <c r="B17" t="s">
-        <v>43</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>77</v>
+      <c r="T16" s="31" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="9"/>
+      <c r="B17" s="36" t="s">
+        <v>37</v>
+      </c>
+      <c r="C17" s="32" t="s">
+        <v>69</v>
       </c>
       <c r="D17" s="1"/>
       <c r="E17" s="1">
@@ -3677,22 +3649,20 @@
       <c r="S17" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="T17" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="18" spans="1:20" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="12">
-        <v>11</v>
-      </c>
-      <c r="B18" t="s">
-        <v>42</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>76</v>
+      <c r="T17" s="31" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A18" s="12"/>
+      <c r="B18" s="36" t="s">
+        <v>61</v>
+      </c>
+      <c r="C18" s="31" t="s">
+        <v>73</v>
       </c>
       <c r="D18" s="1"/>
-      <c r="E18" s="1">
+      <c r="E18" s="32">
         <v>1</v>
       </c>
       <c r="F18" s="1" t="s">
@@ -3712,23 +3682,21 @@
       <c r="S18" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="T18" s="1" t="s">
-        <v>52</v>
+      <c r="T18" s="31" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A19" s="12">
-        <v>12</v>
-      </c>
-      <c r="B19" t="s">
-        <v>38</v>
+      <c r="A19" s="12"/>
+      <c r="B19" s="36" t="s">
+        <v>35</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>98</v>
+        <v>70</v>
       </c>
       <c r="D19" s="1"/>
       <c r="E19" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>29</v>
@@ -3747,23 +3715,21 @@
       <c r="S19" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="T19" s="1" t="s">
-        <v>52</v>
+      <c r="T19" s="31" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A20" s="12">
-        <v>13</v>
-      </c>
-      <c r="B20" t="s">
-        <v>41</v>
+      <c r="A20" s="12"/>
+      <c r="B20" s="35" t="s">
+        <v>39</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>99</v>
+        <v>72</v>
       </c>
       <c r="D20" s="1"/>
       <c r="E20" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>29</v>
@@ -3782,58 +3748,55 @@
       <c r="S20" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="T20" s="1" t="s">
-        <v>52</v>
+      <c r="T20" s="31" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A21" s="12">
-        <v>14</v>
-      </c>
-      <c r="B21" t="s">
-        <v>45</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1">
-        <v>10</v>
-      </c>
-      <c r="F21" s="1" t="s">
+      <c r="A21" s="12"/>
+      <c r="B21" s="37" t="s">
+        <v>33</v>
+      </c>
+      <c r="C21" s="33" t="s">
+        <v>71</v>
+      </c>
+      <c r="D21" s="32"/>
+      <c r="E21" s="32">
+        <v>1</v>
+      </c>
+      <c r="F21" s="32" t="s">
         <v>29</v>
       </c>
       <c r="G21" s="13"/>
       <c r="H21" s="12"/>
-      <c r="I21" s="1"/>
-      <c r="J21" s="1"/>
-      <c r="K21" s="1"/>
-      <c r="L21" s="1"/>
-      <c r="M21" s="1"/>
-      <c r="N21" s="1"/>
+      <c r="I21" s="32"/>
+      <c r="J21" s="32"/>
+      <c r="K21" s="32"/>
+      <c r="L21" s="32"/>
+      <c r="M21" s="32"/>
+      <c r="N21" s="32"/>
       <c r="O21" s="13"/>
       <c r="P21" s="12"/>
+      <c r="Q21" s="32"/>
       <c r="R21" s="13"/>
       <c r="S21" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="T21" s="1" t="s">
-        <v>53</v>
+      <c r="T21" s="31" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A22" s="12">
-        <v>15</v>
-      </c>
-      <c r="B22" t="s">
-        <v>100</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>101</v>
+      <c r="A22" s="12"/>
+      <c r="B22" s="36" t="s">
+        <v>36</v>
+      </c>
+      <c r="C22" s="32" t="s">
+        <v>75</v>
       </c>
       <c r="D22" s="1"/>
-      <c r="E22" s="36">
-        <v>10</v>
+      <c r="E22" s="1">
+        <v>3</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>29</v>
@@ -3852,55 +3815,43 @@
       <c r="S22" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="T22" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="23" spans="1:20" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="12">
-        <v>16</v>
-      </c>
-      <c r="B23" s="35" t="s">
+      <c r="T22" s="31" t="s">
         <v>56</v>
       </c>
-      <c r="C23" s="36" t="s">
-        <v>57</v>
-      </c>
-      <c r="D23" s="1"/>
-      <c r="E23" s="36">
-        <v>1</v>
-      </c>
-      <c r="F23" s="36" t="s">
-        <v>29</v>
-      </c>
-      <c r="G23" s="13"/>
-      <c r="H23" s="12"/>
-      <c r="I23" s="36"/>
-      <c r="J23" s="36"/>
-      <c r="K23" s="36"/>
-      <c r="L23" s="36"/>
-      <c r="M23" s="36"/>
-      <c r="N23" s="36"/>
-      <c r="O23" s="13"/>
-      <c r="P23" s="12"/>
-      <c r="Q23" s="36"/>
-      <c r="R23" s="13"/>
-      <c r="S23" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="T23" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A24" s="12">
-        <v>17</v>
-      </c>
-      <c r="B24" t="s">
-        <v>48</v>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A23" s="39"/>
+      <c r="B23" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D23" s="31"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="31"/>
+      <c r="G23" s="40"/>
+      <c r="H23" s="39"/>
+      <c r="I23" s="31"/>
+      <c r="J23" s="31"/>
+      <c r="K23" s="31"/>
+      <c r="L23" s="31"/>
+      <c r="M23" s="31"/>
+      <c r="N23" s="31"/>
+      <c r="O23" s="40"/>
+      <c r="P23" s="39"/>
+      <c r="Q23" s="31"/>
+      <c r="R23" s="40"/>
+      <c r="S23" s="41"/>
+      <c r="T23" s="31"/>
+    </row>
+    <row r="24" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="12"/>
+      <c r="B24" s="36" t="s">
+        <v>77</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D24" s="1"/>
       <c r="E24" s="1">
@@ -3923,58 +3874,55 @@
       <c r="S24" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="T24" s="1" t="s">
-        <v>52</v>
+      <c r="T24" s="31" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A25" s="12">
-        <v>18</v>
-      </c>
-      <c r="B25" t="s">
-        <v>95</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1">
-        <v>1</v>
+      <c r="A25" s="12"/>
+      <c r="B25" s="37" t="s">
+        <v>32</v>
+      </c>
+      <c r="C25" s="32" t="s">
+        <v>79</v>
+      </c>
+      <c r="D25" s="32"/>
+      <c r="E25" s="32">
+        <v>10</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>29</v>
       </c>
       <c r="G25" s="13"/>
       <c r="H25" s="12"/>
-      <c r="I25" s="1"/>
-      <c r="J25" s="1"/>
-      <c r="K25" s="1"/>
-      <c r="L25" s="1"/>
-      <c r="M25" s="1"/>
-      <c r="N25" s="1"/>
+      <c r="I25" s="32"/>
+      <c r="J25" s="32"/>
+      <c r="K25" s="32"/>
+      <c r="L25" s="32"/>
+      <c r="M25" s="32"/>
+      <c r="N25" s="32"/>
       <c r="O25" s="13"/>
       <c r="P25" s="12"/>
+      <c r="Q25" s="32"/>
       <c r="R25" s="13"/>
       <c r="S25" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="T25" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A26" s="12">
-        <v>19</v>
-      </c>
-      <c r="B26" s="32" t="s">
-        <v>32</v>
-      </c>
-      <c r="C26" s="37" t="s">
-        <v>75</v>
+      <c r="T25" s="31" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="12"/>
+      <c r="B26" s="35" t="s">
+        <v>42</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>80</v>
       </c>
       <c r="D26" s="1"/>
       <c r="E26" s="1">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>29</v>
@@ -3993,19 +3941,17 @@
       <c r="S26" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="T26" s="1" t="s">
+      <c r="T26" s="31" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A27" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="B27" t="s">
-        <v>46</v>
-      </c>
-      <c r="C27" s="36" t="s">
-        <v>61</v>
+      <c r="A27" s="12"/>
+      <c r="B27" s="35" t="s">
+        <v>43</v>
+      </c>
+      <c r="C27" s="32" t="s">
+        <v>81</v>
       </c>
       <c r="D27" s="1"/>
       <c r="E27" s="1">
@@ -4028,23 +3974,21 @@
       <c r="S27" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="T27" s="1" t="s">
-        <v>53</v>
+      <c r="T27" s="31" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A28" s="12" t="s">
-        <v>105</v>
-      </c>
-      <c r="B28" t="s">
-        <v>44</v>
+      <c r="A28" s="12"/>
+      <c r="B28" s="35" t="s">
+        <v>51</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>62</v>
+        <v>82</v>
       </c>
       <c r="D28" s="1"/>
       <c r="E28" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F28" s="1" t="s">
         <v>29</v>
@@ -4063,23 +4007,21 @@
       <c r="S28" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="T28" s="1" t="s">
-        <v>53</v>
+      <c r="T28" s="31" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A29" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="B29" t="s">
-        <v>47</v>
-      </c>
-      <c r="C29" s="33" t="s">
-        <v>94</v>
+      <c r="A29" s="12"/>
+      <c r="B29" s="35" t="s">
+        <v>83</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>84</v>
       </c>
       <c r="D29" s="1"/>
       <c r="E29" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F29" s="1" t="s">
         <v>29</v>
@@ -4098,19 +4040,17 @@
       <c r="S29" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="T29" s="1" t="s">
-        <v>53</v>
+      <c r="T29" s="31" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A30" s="12" t="s">
-        <v>106</v>
-      </c>
-      <c r="B30" t="s">
-        <v>40</v>
-      </c>
-      <c r="C30" s="33" t="s">
-        <v>93</v>
+      <c r="A30" s="12"/>
+      <c r="B30" s="35" t="s">
+        <v>48</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>85</v>
       </c>
       <c r="D30" s="1"/>
       <c r="E30" s="1">
@@ -4133,23 +4073,19 @@
       <c r="S30" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="T30" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="31" spans="1:20" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="12" t="s">
-        <v>104</v>
-      </c>
-      <c r="B31" t="s">
-        <v>58</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>60</v>
-      </c>
+      <c r="T30" s="31" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A31" s="12"/>
+      <c r="B31" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="C31" s="1"/>
       <c r="D31" s="1"/>
-      <c r="E31" s="36">
-        <v>1</v>
+      <c r="E31" s="1">
+        <v>5</v>
       </c>
       <c r="F31" s="1" t="s">
         <v>29</v>
@@ -4168,20 +4104,16 @@
       <c r="S31" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="T31" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="32" spans="1:20" ht="30" x14ac:dyDescent="0.25">
-      <c r="A32" s="12" t="s">
-        <v>107</v>
-      </c>
-      <c r="B32" t="s">
-        <v>49</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>64</v>
-      </c>
+      <c r="T31" s="31" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A32" s="12"/>
+      <c r="B32" s="35" t="s">
+        <v>38</v>
+      </c>
+      <c r="C32" s="32"/>
       <c r="D32" s="1"/>
       <c r="E32" s="1">
         <v>5</v>
@@ -4203,13 +4135,13 @@
       <c r="S32" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="T32" s="1" t="s">
-        <v>53</v>
+      <c r="T32" s="31" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="33" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A33" s="12"/>
-      <c r="B33" s="1"/>
+      <c r="B33" s="31"/>
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
@@ -4228,7 +4160,7 @@
       <c r="S33" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="T33" s="1"/>
+      <c r="T33" s="31"/>
     </row>
     <row r="34" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
@@ -4271,7 +4203,7 @@
     <row r="36" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="1" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
@@ -4292,7 +4224,7 @@
     <row r="37" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" s="1" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
@@ -4313,10 +4245,10 @@
     <row r="38" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="1" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
@@ -4336,7 +4268,7 @@
     <row r="39" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="B39" s="1" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
@@ -4357,10 +4289,10 @@
     <row r="40" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="B40" s="1" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="D40" s="1"/>
       <c r="E40" s="1"/>
@@ -4380,10 +4312,10 @@
     <row r="41" spans="1:20" ht="45" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="B41" s="1" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="D41" s="1"/>
       <c r="E41" s="1"/>
@@ -4403,10 +4335,10 @@
     <row r="42" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
       <c r="B42" s="1" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="D42" s="1"/>
       <c r="E42" s="1"/>
@@ -4426,10 +4358,10 @@
     <row r="43" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
       <c r="B43" s="1" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D43" s="1"/>
       <c r="E43" s="1"/>
@@ -4449,7 +4381,7 @@
     <row r="44" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
       <c r="B44" s="1" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="C44" s="1"/>
       <c r="D44" s="1"/>
@@ -4470,7 +4402,7 @@
     <row r="45" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
       <c r="B45" s="1" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>

</xml_diff>

<commit_message>
Reapply "Merge branch 'main' of https://github.com/HKiet-dev/G4U"
This reverts commit 53a02fd60a4db9522afdfa4e2a07c7e436301468.
</commit_message>
<xml_diff>
--- a/Report/Requirement (1).xlsx
+++ b/Report/Requirement (1).xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28014"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28105"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FPT Polytechnic\Graduation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FPT Polytechnic\Graduation\G4U\Report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55799C48-460A-454D-82DA-2AF184663F1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B79ECDD3-61AC-4C76-B310-E6F2B047903F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{66551FA1-06BE-4D31-8093-516AC48B2C2B}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="108">
   <si>
     <t>Requirements Description</t>
   </si>
@@ -195,12 +195,6 @@
     <t>Thống kê (in pdf, excel)</t>
   </si>
   <si>
-    <t>Báo cáo game</t>
-  </si>
-  <si>
-    <t>Thanh toán (momo, vnpay, COD)</t>
-  </si>
-  <si>
     <t>Role</t>
   </si>
   <si>
@@ -243,9 +237,6 @@
     <t>Kiệt</t>
   </si>
   <si>
-    <t>Đang tìm hiểu...</t>
-  </si>
-  <si>
     <t>Thống kế số lượng, số lượng chơi game từng sp,…. Có in file excel, pdf</t>
   </si>
   <si>
@@ -267,9 +258,6 @@
     <t>Đăng nhập đăng kí tài khoản bình thường</t>
   </si>
   <si>
-    <t>Báo cáo game không phù hợp, game lỗi</t>
-  </si>
-  <si>
     <t>Lọc theo thể loại, theo tuổi, theo giá</t>
   </si>
   <si>
@@ -291,15 +279,9 @@
     <t>down bằng link của ggdrive với terrabox</t>
   </si>
   <si>
-    <t>lấy c#6 ra mà làm</t>
-  </si>
-  <si>
     <t>Xem, chỉnh sửa hồ sơ, đổi mk</t>
   </si>
   <si>
-    <t>tương tự</t>
-  </si>
-  <si>
     <t>Hiện thời gian, trạng thái, sản phẩm đã mua</t>
   </si>
   <si>
@@ -340,6 +322,51 @@
   </si>
   <si>
     <t>Tần, Hưng, Nhân</t>
+  </si>
+  <si>
+    <t>Đưa hình ảnh lên AI kiểm tra</t>
+  </si>
+  <si>
+    <t>Dùng Google Adsense</t>
+  </si>
+  <si>
+    <t>Thanh toán (momo, vpn)</t>
+  </si>
+  <si>
+    <t>Thanh toán qua các hình thức online banking</t>
+  </si>
+  <si>
+    <t>Chỉnh sửa thông tin cá nhân: tên hiển thị, avatar, số điện thoại</t>
+  </si>
+  <si>
+    <t>Thêm sản phẩm yêu thích vào wishlist</t>
+  </si>
+  <si>
+    <t>Thêm xóa sửa các sản phẩm yêu thích</t>
+  </si>
+  <si>
+    <t>Tố cáo game</t>
+  </si>
+  <si>
+    <t>Tố cáo game không phù hợp, game lỗi</t>
+  </si>
+  <si>
+    <t>Admin-1</t>
+  </si>
+  <si>
+    <t>Admin-3</t>
+  </si>
+  <si>
+    <t>Admin-5</t>
+  </si>
+  <si>
+    <t>Admin-2</t>
+  </si>
+  <si>
+    <t>Admin-4</t>
+  </si>
+  <si>
+    <t>Admin-6</t>
   </si>
 </sst>
 </file>
@@ -397,9 +424,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -585,7 +610,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -640,6 +665,7 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -673,29 +699,18 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1078,7 +1093,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:pivotSource>
-    <c:name>[Requirement.xlsx]Status!PivotTable5</c:name>
+    <c:name>[Requirement (1).xlsx]Status!PivotTable5</c:name>
     <c:fmtId val="0"/>
   </c:pivotSource>
   <c:chart>
@@ -2760,7 +2775,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D670A074-11C2-4534-81DA-C65028B9F80D}" name="Table2" displayName="Table2" ref="A7:T33" totalsRowShown="0" headerRowDxfId="32" dataDxfId="31">
   <autoFilter ref="A7:T33" xr:uid="{40ACC06F-DF0F-4565-AB81-61F9F81BAAF1}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A8:T33">
-    <sortCondition ref="T7:T33"/>
+    <sortCondition ref="A7:A33"/>
   </sortState>
   <tableColumns count="20">
     <tableColumn id="1" xr3:uid="{64031A45-824B-4700-8A01-8F0F87C05385}" name="Req. ID" dataDxfId="30"/>
@@ -3087,8 +3102,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7551B106-1BC4-4794-8DF3-1BDFDAFF6E5D}">
   <dimension ref="A1:V321"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B47" sqref="B47"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3130,11 +3145,11 @@
       <c r="P1" s="4"/>
       <c r="Q1" s="5"/>
       <c r="R1" s="4"/>
-      <c r="T1" s="20" t="s">
+      <c r="T1" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="U1" s="20"/>
-      <c r="V1" s="20"/>
+      <c r="U1" s="21"/>
+      <c r="V1" s="21"/>
     </row>
     <row r="2" spans="1:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
@@ -3155,11 +3170,11 @@
       <c r="P2" s="4"/>
       <c r="Q2" s="5"/>
       <c r="R2" s="4"/>
-      <c r="T2" s="21" t="s">
+      <c r="T2" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="U2" s="21"/>
-      <c r="V2" s="21"/>
+      <c r="U2" s="22"/>
+      <c r="V2" s="22"/>
     </row>
     <row r="3" spans="1:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
@@ -3168,57 +3183,57 @@
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
-      <c r="G3" s="30" t="s">
+      <c r="G3" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="H3" s="30"/>
-      <c r="I3" s="30"/>
-      <c r="J3" s="30"/>
-      <c r="K3" s="30"/>
-      <c r="L3" s="30"/>
-      <c r="M3" s="30"/>
-      <c r="N3" s="30"/>
-      <c r="O3" s="30"/>
+      <c r="H3" s="31"/>
+      <c r="I3" s="31"/>
+      <c r="J3" s="31"/>
+      <c r="K3" s="31"/>
+      <c r="L3" s="31"/>
+      <c r="M3" s="31"/>
+      <c r="N3" s="31"/>
+      <c r="O3" s="31"/>
       <c r="P3" s="4"/>
       <c r="Q3" s="5"/>
       <c r="R3" s="4"/>
-      <c r="T3" s="21" t="s">
+      <c r="T3" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="U3" s="21"/>
-      <c r="V3" s="21"/>
+      <c r="U3" s="22"/>
+      <c r="V3" s="22"/>
     </row>
     <row r="4" spans="1:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="27"/>
-      <c r="C4" s="28" t="s">
+      <c r="B4" s="28"/>
+      <c r="C4" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="D4" s="29"/>
+      <c r="D4" s="30"/>
       <c r="E4" s="19"/>
       <c r="F4" s="4"/>
-      <c r="G4" s="30"/>
-      <c r="H4" s="30"/>
-      <c r="I4" s="30"/>
-      <c r="J4" s="30"/>
-      <c r="K4" s="30"/>
-      <c r="L4" s="30"/>
-      <c r="M4" s="30"/>
-      <c r="N4" s="30"/>
-      <c r="O4" s="30"/>
+      <c r="G4" s="31"/>
+      <c r="H4" s="31"/>
+      <c r="I4" s="31"/>
+      <c r="J4" s="31"/>
+      <c r="K4" s="31"/>
+      <c r="L4" s="31"/>
+      <c r="M4" s="31"/>
+      <c r="N4" s="31"/>
+      <c r="O4" s="31"/>
       <c r="P4" s="4"/>
       <c r="Q4" s="5"/>
       <c r="R4" s="4"/>
     </row>
     <row r="5" spans="1:22" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="26" t="s">
+      <c r="A5" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="26"/>
-      <c r="C5" s="28"/>
-      <c r="D5" s="29"/>
+      <c r="B5" s="27"/>
+      <c r="C5" s="29"/>
+      <c r="D5" s="30"/>
       <c r="E5" s="19"/>
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
@@ -3235,29 +3250,29 @@
       <c r="R5" s="4"/>
     </row>
     <row r="6" spans="1:22" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="22" t="s">
+      <c r="A6" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="23"/>
-      <c r="C6" s="24"/>
-      <c r="D6" s="24"/>
-      <c r="E6" s="24"/>
-      <c r="F6" s="25"/>
-      <c r="G6" s="22" t="s">
+      <c r="B6" s="24"/>
+      <c r="C6" s="25"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="25"/>
+      <c r="F6" s="26"/>
+      <c r="G6" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="H6" s="23"/>
-      <c r="I6" s="23"/>
-      <c r="J6" s="23"/>
-      <c r="K6" s="23"/>
-      <c r="L6" s="23"/>
-      <c r="M6" s="23"/>
-      <c r="N6" s="25"/>
-      <c r="O6" s="22" t="s">
+      <c r="H6" s="24"/>
+      <c r="I6" s="24"/>
+      <c r="J6" s="24"/>
+      <c r="K6" s="24"/>
+      <c r="L6" s="24"/>
+      <c r="M6" s="24"/>
+      <c r="N6" s="26"/>
+      <c r="O6" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="P6" s="23"/>
-      <c r="Q6" s="25"/>
+      <c r="P6" s="24"/>
+      <c r="Q6" s="26"/>
       <c r="R6" s="3"/>
     </row>
     <row r="7" spans="1:22" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
@@ -3319,16 +3334,18 @@
         <v>12</v>
       </c>
       <c r="T7" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="8" spans="1:22" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="9"/>
-      <c r="B8" s="34" t="s">
-        <v>58</v>
-      </c>
-      <c r="C8" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A8" s="9">
+        <v>1</v>
+      </c>
+      <c r="B8" s="20" t="s">
         <v>59</v>
+      </c>
+      <c r="C8" s="36" t="s">
+        <v>70</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="10">
@@ -3352,21 +3369,23 @@
       <c r="S8" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="T8" s="31" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="9" spans="1:22" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="12"/>
-      <c r="B9" s="35" t="s">
-        <v>60</v>
+      <c r="T8" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A9" s="12">
+        <v>2</v>
+      </c>
+      <c r="B9" t="s">
+        <v>39</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="D9" s="31"/>
+        <v>69</v>
+      </c>
+      <c r="D9" s="1"/>
       <c r="E9" s="10">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>29</v>
@@ -3385,17 +3404,19 @@
       <c r="S9" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="T9" s="31" t="s">
-        <v>55</v>
+      <c r="T9" s="1" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A10" s="9"/>
-      <c r="B10" s="35" t="s">
-        <v>46</v>
+      <c r="A10" s="9">
+        <v>3</v>
+      </c>
+      <c r="B10" t="s">
+        <v>37</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1">
@@ -3418,21 +3439,23 @@
       <c r="S10" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="T10" s="31" t="s">
+      <c r="T10" s="1" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A11" s="12"/>
-      <c r="B11" s="35" t="s">
-        <v>44</v>
+      <c r="A11" s="12">
+        <v>4</v>
+      </c>
+      <c r="B11" t="s">
+        <v>35</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>29</v>
@@ -3451,21 +3474,23 @@
       <c r="S11" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="T11" s="31" t="s">
-        <v>55</v>
+      <c r="T11" s="1" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A12" s="9"/>
-      <c r="B12" s="35" t="s">
-        <v>40</v>
-      </c>
-      <c r="C12" s="38" t="s">
-        <v>66</v>
+      <c r="A12" s="9">
+        <v>5</v>
+      </c>
+      <c r="B12" t="s">
+        <v>78</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>97</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>29</v>
@@ -3484,58 +3509,59 @@
       <c r="S12" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="T12" s="31" t="s">
-        <v>55</v>
+      <c r="T12" s="1" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A13" s="12"/>
+      <c r="A13" s="12">
+        <v>6</v>
+      </c>
       <c r="B13" s="35" t="s">
-        <v>47</v>
-      </c>
-      <c r="C13" s="38" t="s">
-        <v>66</v>
+        <v>33</v>
+      </c>
+      <c r="C13" s="34" t="s">
+        <v>68</v>
       </c>
       <c r="D13" s="1"/>
-      <c r="E13" s="1">
-        <v>4</v>
-      </c>
-      <c r="F13" s="1" t="s">
+      <c r="E13" s="36">
+        <v>1</v>
+      </c>
+      <c r="F13" s="36" t="s">
         <v>29</v>
       </c>
       <c r="G13" s="13"/>
       <c r="H13" s="12"/>
-      <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
-      <c r="K13" s="1"/>
-      <c r="L13" s="1"/>
-      <c r="M13" s="1"/>
-      <c r="N13" s="1"/>
+      <c r="I13" s="36"/>
+      <c r="J13" s="36"/>
+      <c r="K13" s="36"/>
+      <c r="L13" s="36"/>
+      <c r="M13" s="36"/>
+      <c r="N13" s="36"/>
       <c r="O13" s="13"/>
       <c r="P13" s="12"/>
+      <c r="Q13" s="36"/>
       <c r="R13" s="13"/>
       <c r="S13" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="T13" s="31" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="14" spans="1:22" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="9"/>
-      <c r="B14" s="35" t="s">
-        <v>49</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>67</v>
+      <c r="T13" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A14" s="9">
+        <v>7</v>
+      </c>
+      <c r="B14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" s="36" t="s">
+        <v>72</v>
       </c>
       <c r="D14" s="1"/>
-      <c r="E14" s="1">
-        <v>5</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>29</v>
-      </c>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
       <c r="G14" s="13"/>
       <c r="H14" s="12"/>
       <c r="I14" s="1"/>
@@ -3547,24 +3573,22 @@
       <c r="O14" s="13"/>
       <c r="P14" s="12"/>
       <c r="R14" s="13"/>
-      <c r="S14" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="T14" s="31" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A15" s="12"/>
-      <c r="B15" s="35" t="s">
-        <v>45</v>
+      <c r="S14" s="17"/>
+      <c r="T14" s="1"/>
+    </row>
+    <row r="15" spans="1:22" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="12">
+        <v>8</v>
+      </c>
+      <c r="B15" t="s">
+        <v>73</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="D15" s="1"/>
-      <c r="E15" s="32">
-        <v>10</v>
+      <c r="E15" s="1">
+        <v>3</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>29</v>
@@ -3583,21 +3607,23 @@
       <c r="S15" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="T15" s="31" t="s">
-        <v>55</v>
+      <c r="T15" s="1" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A16" s="12"/>
-      <c r="B16" s="35" t="s">
-        <v>50</v>
-      </c>
-      <c r="C16" s="32" t="s">
-        <v>74</v>
+      <c r="A16" s="12">
+        <v>9</v>
+      </c>
+      <c r="B16" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>71</v>
       </c>
       <c r="D16" s="1"/>
       <c r="E16" s="1">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>29</v>
@@ -3616,17 +3642,19 @@
       <c r="S16" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="T16" s="31" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="17" spans="1:20" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="9"/>
-      <c r="B17" s="36" t="s">
-        <v>37</v>
-      </c>
-      <c r="C17" s="32" t="s">
-        <v>69</v>
+      <c r="T16" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A17" s="9">
+        <v>10</v>
+      </c>
+      <c r="B17" t="s">
+        <v>43</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>77</v>
       </c>
       <c r="D17" s="1"/>
       <c r="E17" s="1">
@@ -3649,20 +3677,22 @@
       <c r="S17" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="T17" s="31" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A18" s="12"/>
-      <c r="B18" s="36" t="s">
-        <v>61</v>
-      </c>
-      <c r="C18" s="31" t="s">
-        <v>73</v>
+      <c r="T17" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="12">
+        <v>11</v>
+      </c>
+      <c r="B18" t="s">
+        <v>42</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>76</v>
       </c>
       <c r="D18" s="1"/>
-      <c r="E18" s="32">
+      <c r="E18" s="1">
         <v>1</v>
       </c>
       <c r="F18" s="1" t="s">
@@ -3682,21 +3712,23 @@
       <c r="S18" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="T18" s="31" t="s">
-        <v>53</v>
+      <c r="T18" s="1" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A19" s="12"/>
-      <c r="B19" s="36" t="s">
-        <v>35</v>
+      <c r="A19" s="12">
+        <v>12</v>
+      </c>
+      <c r="B19" t="s">
+        <v>38</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>70</v>
+        <v>98</v>
       </c>
       <c r="D19" s="1"/>
       <c r="E19" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>29</v>
@@ -3715,21 +3747,23 @@
       <c r="S19" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="T19" s="31" t="s">
-        <v>53</v>
+      <c r="T19" s="1" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A20" s="12"/>
-      <c r="B20" s="35" t="s">
-        <v>39</v>
+      <c r="A20" s="12">
+        <v>13</v>
+      </c>
+      <c r="B20" t="s">
+        <v>41</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>72</v>
+        <v>99</v>
       </c>
       <c r="D20" s="1"/>
       <c r="E20" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>29</v>
@@ -3748,55 +3782,58 @@
       <c r="S20" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="T20" s="31" t="s">
-        <v>53</v>
+      <c r="T20" s="1" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A21" s="12"/>
-      <c r="B21" s="37" t="s">
-        <v>33</v>
-      </c>
-      <c r="C21" s="33" t="s">
-        <v>71</v>
-      </c>
-      <c r="D21" s="32"/>
-      <c r="E21" s="32">
-        <v>1</v>
-      </c>
-      <c r="F21" s="32" t="s">
+      <c r="A21" s="12">
+        <v>14</v>
+      </c>
+      <c r="B21" t="s">
+        <v>45</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1">
+        <v>10</v>
+      </c>
+      <c r="F21" s="1" t="s">
         <v>29</v>
       </c>
       <c r="G21" s="13"/>
       <c r="H21" s="12"/>
-      <c r="I21" s="32"/>
-      <c r="J21" s="32"/>
-      <c r="K21" s="32"/>
-      <c r="L21" s="32"/>
-      <c r="M21" s="32"/>
-      <c r="N21" s="32"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+      <c r="K21" s="1"/>
+      <c r="L21" s="1"/>
+      <c r="M21" s="1"/>
+      <c r="N21" s="1"/>
       <c r="O21" s="13"/>
       <c r="P21" s="12"/>
-      <c r="Q21" s="32"/>
       <c r="R21" s="13"/>
       <c r="S21" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="T21" s="31" t="s">
-        <v>56</v>
+      <c r="T21" s="1" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A22" s="12"/>
-      <c r="B22" s="36" t="s">
-        <v>36</v>
-      </c>
-      <c r="C22" s="32" t="s">
-        <v>75</v>
+      <c r="A22" s="12">
+        <v>15</v>
+      </c>
+      <c r="B22" t="s">
+        <v>100</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>101</v>
       </c>
       <c r="D22" s="1"/>
-      <c r="E22" s="1">
-        <v>3</v>
+      <c r="E22" s="36">
+        <v>10</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>29</v>
@@ -3815,43 +3852,55 @@
       <c r="S22" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="T22" s="31" t="s">
+      <c r="T22" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="12">
+        <v>16</v>
+      </c>
+      <c r="B23" s="35" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A23" s="39"/>
-      <c r="B23" s="36" t="s">
-        <v>34</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="D23" s="31"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="31"/>
-      <c r="G23" s="40"/>
-      <c r="H23" s="39"/>
-      <c r="I23" s="31"/>
-      <c r="J23" s="31"/>
-      <c r="K23" s="31"/>
-      <c r="L23" s="31"/>
-      <c r="M23" s="31"/>
-      <c r="N23" s="31"/>
-      <c r="O23" s="40"/>
-      <c r="P23" s="39"/>
-      <c r="Q23" s="31"/>
-      <c r="R23" s="40"/>
-      <c r="S23" s="41"/>
-      <c r="T23" s="31"/>
-    </row>
-    <row r="24" spans="1:20" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="12"/>
-      <c r="B24" s="36" t="s">
-        <v>77</v>
+      <c r="C23" s="36" t="s">
+        <v>57</v>
+      </c>
+      <c r="D23" s="1"/>
+      <c r="E23" s="36">
+        <v>1</v>
+      </c>
+      <c r="F23" s="36" t="s">
+        <v>29</v>
+      </c>
+      <c r="G23" s="13"/>
+      <c r="H23" s="12"/>
+      <c r="I23" s="36"/>
+      <c r="J23" s="36"/>
+      <c r="K23" s="36"/>
+      <c r="L23" s="36"/>
+      <c r="M23" s="36"/>
+      <c r="N23" s="36"/>
+      <c r="O23" s="13"/>
+      <c r="P23" s="12"/>
+      <c r="Q23" s="36"/>
+      <c r="R23" s="13"/>
+      <c r="S23" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="T23" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A24" s="12">
+        <v>17</v>
+      </c>
+      <c r="B24" t="s">
+        <v>48</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D24" s="1"/>
       <c r="E24" s="1">
@@ -3874,55 +3923,58 @@
       <c r="S24" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="T24" s="31" t="s">
-        <v>56</v>
+      <c r="T24" s="1" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A25" s="12"/>
-      <c r="B25" s="37" t="s">
-        <v>32</v>
-      </c>
-      <c r="C25" s="32" t="s">
-        <v>79</v>
-      </c>
-      <c r="D25" s="32"/>
-      <c r="E25" s="32">
-        <v>10</v>
+      <c r="A25" s="12">
+        <v>18</v>
+      </c>
+      <c r="B25" t="s">
+        <v>95</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1">
+        <v>1</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>29</v>
       </c>
       <c r="G25" s="13"/>
       <c r="H25" s="12"/>
-      <c r="I25" s="32"/>
-      <c r="J25" s="32"/>
-      <c r="K25" s="32"/>
-      <c r="L25" s="32"/>
-      <c r="M25" s="32"/>
-      <c r="N25" s="32"/>
+      <c r="I25" s="1"/>
+      <c r="J25" s="1"/>
+      <c r="K25" s="1"/>
+      <c r="L25" s="1"/>
+      <c r="M25" s="1"/>
+      <c r="N25" s="1"/>
       <c r="O25" s="13"/>
       <c r="P25" s="12"/>
-      <c r="Q25" s="32"/>
       <c r="R25" s="13"/>
       <c r="S25" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="T25" s="31" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="26" spans="1:20" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="12"/>
-      <c r="B26" s="35" t="s">
-        <v>42</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>80</v>
+      <c r="T25" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A26" s="12">
+        <v>19</v>
+      </c>
+      <c r="B26" s="32" t="s">
+        <v>32</v>
+      </c>
+      <c r="C26" s="37" t="s">
+        <v>75</v>
       </c>
       <c r="D26" s="1"/>
       <c r="E26" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>29</v>
@@ -3941,17 +3993,19 @@
       <c r="S26" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="T26" s="31" t="s">
+      <c r="T26" s="1" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A27" s="12"/>
-      <c r="B27" s="35" t="s">
-        <v>43</v>
-      </c>
-      <c r="C27" s="32" t="s">
-        <v>81</v>
+      <c r="A27" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="B27" t="s">
+        <v>46</v>
+      </c>
+      <c r="C27" s="36" t="s">
+        <v>61</v>
       </c>
       <c r="D27" s="1"/>
       <c r="E27" s="1">
@@ -3974,21 +4028,23 @@
       <c r="S27" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="T27" s="31" t="s">
-        <v>54</v>
+      <c r="T27" s="1" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A28" s="12"/>
-      <c r="B28" s="35" t="s">
-        <v>51</v>
+      <c r="A28" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="B28" t="s">
+        <v>44</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>82</v>
+        <v>62</v>
       </c>
       <c r="D28" s="1"/>
       <c r="E28" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F28" s="1" t="s">
         <v>29</v>
@@ -4007,21 +4063,23 @@
       <c r="S28" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="T28" s="31" t="s">
-        <v>54</v>
+      <c r="T28" s="1" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A29" s="12"/>
-      <c r="B29" s="35" t="s">
-        <v>83</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>84</v>
+      <c r="A29" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="B29" t="s">
+        <v>47</v>
+      </c>
+      <c r="C29" s="33" t="s">
+        <v>94</v>
       </c>
       <c r="D29" s="1"/>
       <c r="E29" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F29" s="1" t="s">
         <v>29</v>
@@ -4040,17 +4098,19 @@
       <c r="S29" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="T29" s="31" t="s">
-        <v>54</v>
+      <c r="T29" s="1" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A30" s="12"/>
-      <c r="B30" s="35" t="s">
-        <v>48</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>85</v>
+      <c r="A30" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="B30" t="s">
+        <v>40</v>
+      </c>
+      <c r="C30" s="33" t="s">
+        <v>93</v>
       </c>
       <c r="D30" s="1"/>
       <c r="E30" s="1">
@@ -4073,19 +4133,23 @@
       <c r="S30" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="T30" s="31" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A31" s="12"/>
-      <c r="B31" s="35" t="s">
-        <v>41</v>
-      </c>
-      <c r="C31" s="1"/>
+      <c r="T30" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="31" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+      <c r="A31" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="B31" t="s">
+        <v>58</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>60</v>
+      </c>
       <c r="D31" s="1"/>
-      <c r="E31" s="1">
-        <v>5</v>
+      <c r="E31" s="36">
+        <v>1</v>
       </c>
       <c r="F31" s="1" t="s">
         <v>29</v>
@@ -4104,16 +4168,20 @@
       <c r="S31" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="T31" s="31" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A32" s="12"/>
-      <c r="B32" s="35" t="s">
-        <v>38</v>
-      </c>
-      <c r="C32" s="32"/>
+      <c r="T31" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="32" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+      <c r="A32" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="B32" t="s">
+        <v>49</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>64</v>
+      </c>
       <c r="D32" s="1"/>
       <c r="E32" s="1">
         <v>5</v>
@@ -4135,13 +4203,13 @@
       <c r="S32" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="T32" s="31" t="s">
-        <v>54</v>
+      <c r="T32" s="1" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="33" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A33" s="12"/>
-      <c r="B33" s="31"/>
+      <c r="B33" s="1"/>
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
@@ -4160,7 +4228,7 @@
       <c r="S33" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="T33" s="31"/>
+      <c r="T33" s="1"/>
     </row>
     <row r="34" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
@@ -4203,7 +4271,7 @@
     <row r="36" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="1" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
@@ -4224,7 +4292,7 @@
     <row r="37" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" s="1" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
@@ -4245,10 +4313,10 @@
     <row r="38" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="1" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
@@ -4268,7 +4336,7 @@
     <row r="39" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="B39" s="1" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
@@ -4289,10 +4357,10 @@
     <row r="40" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="B40" s="1" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="D40" s="1"/>
       <c r="E40" s="1"/>
@@ -4312,10 +4380,10 @@
     <row r="41" spans="1:20" ht="45" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="B41" s="1" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="D41" s="1"/>
       <c r="E41" s="1"/>
@@ -4335,10 +4403,10 @@
     <row r="42" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
       <c r="B42" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C42" s="1" t="s">
         <v>92</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>98</v>
       </c>
       <c r="D42" s="1"/>
       <c r="E42" s="1"/>
@@ -4358,10 +4426,10 @@
     <row r="43" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
       <c r="B43" s="1" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D43" s="1"/>
       <c r="E43" s="1"/>
@@ -4381,7 +4449,7 @@
     <row r="44" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
       <c r="B44" s="1" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="C44" s="1"/>
       <c r="D44" s="1"/>
@@ -4402,7 +4470,7 @@
     <row r="45" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
       <c r="B45" s="1" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>

</xml_diff>

<commit_message>
Revert "Reapply "Merge branch 'main' of https://github.com/HKiet-dev/G4U""
This reverts commit 925ac4ec8f7cd6c8183523d883e9f7c7afe56721.
</commit_message>
<xml_diff>
--- a/Report/Requirement (1).xlsx
+++ b/Report/Requirement (1).xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28105"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28014"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FPT Polytechnic\Graduation\G4U\Report\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FPT Polytechnic\Graduation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B79ECDD3-61AC-4C76-B310-E6F2B047903F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55799C48-460A-454D-82DA-2AF184663F1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{66551FA1-06BE-4D31-8093-516AC48B2C2B}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="99">
   <si>
     <t>Requirements Description</t>
   </si>
@@ -195,6 +195,12 @@
     <t>Thống kê (in pdf, excel)</t>
   </si>
   <si>
+    <t>Báo cáo game</t>
+  </si>
+  <si>
+    <t>Thanh toán (momo, vnpay, COD)</t>
+  </si>
+  <si>
     <t>Role</t>
   </si>
   <si>
@@ -237,6 +243,9 @@
     <t>Kiệt</t>
   </si>
   <si>
+    <t>Đang tìm hiểu...</t>
+  </si>
+  <si>
     <t>Thống kế số lượng, số lượng chơi game từng sp,…. Có in file excel, pdf</t>
   </si>
   <si>
@@ -258,6 +267,9 @@
     <t>Đăng nhập đăng kí tài khoản bình thường</t>
   </si>
   <si>
+    <t>Báo cáo game không phù hợp, game lỗi</t>
+  </si>
+  <si>
     <t>Lọc theo thể loại, theo tuổi, theo giá</t>
   </si>
   <si>
@@ -279,9 +291,15 @@
     <t>down bằng link của ggdrive với terrabox</t>
   </si>
   <si>
+    <t>lấy c#6 ra mà làm</t>
+  </si>
+  <si>
     <t>Xem, chỉnh sửa hồ sơ, đổi mk</t>
   </si>
   <si>
+    <t>tương tự</t>
+  </si>
+  <si>
     <t>Hiện thời gian, trạng thái, sản phẩm đã mua</t>
   </si>
   <si>
@@ -322,51 +340,6 @@
   </si>
   <si>
     <t>Tần, Hưng, Nhân</t>
-  </si>
-  <si>
-    <t>Đưa hình ảnh lên AI kiểm tra</t>
-  </si>
-  <si>
-    <t>Dùng Google Adsense</t>
-  </si>
-  <si>
-    <t>Thanh toán (momo, vpn)</t>
-  </si>
-  <si>
-    <t>Thanh toán qua các hình thức online banking</t>
-  </si>
-  <si>
-    <t>Chỉnh sửa thông tin cá nhân: tên hiển thị, avatar, số điện thoại</t>
-  </si>
-  <si>
-    <t>Thêm sản phẩm yêu thích vào wishlist</t>
-  </si>
-  <si>
-    <t>Thêm xóa sửa các sản phẩm yêu thích</t>
-  </si>
-  <si>
-    <t>Tố cáo game</t>
-  </si>
-  <si>
-    <t>Tố cáo game không phù hợp, game lỗi</t>
-  </si>
-  <si>
-    <t>Admin-1</t>
-  </si>
-  <si>
-    <t>Admin-3</t>
-  </si>
-  <si>
-    <t>Admin-5</t>
-  </si>
-  <si>
-    <t>Admin-2</t>
-  </si>
-  <si>
-    <t>Admin-4</t>
-  </si>
-  <si>
-    <t>Admin-6</t>
   </si>
 </sst>
 </file>
@@ -424,7 +397,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -610,7 +585,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -665,7 +640,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -699,18 +673,29 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1093,7 +1078,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:pivotSource>
-    <c:name>[Requirement (1).xlsx]Status!PivotTable5</c:name>
+    <c:name>[Requirement.xlsx]Status!PivotTable5</c:name>
     <c:fmtId val="0"/>
   </c:pivotSource>
   <c:chart>
@@ -2775,7 +2760,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D670A074-11C2-4534-81DA-C65028B9F80D}" name="Table2" displayName="Table2" ref="A7:T33" totalsRowShown="0" headerRowDxfId="32" dataDxfId="31">
   <autoFilter ref="A7:T33" xr:uid="{40ACC06F-DF0F-4565-AB81-61F9F81BAAF1}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A8:T33">
-    <sortCondition ref="A7:A33"/>
+    <sortCondition ref="T7:T33"/>
   </sortState>
   <tableColumns count="20">
     <tableColumn id="1" xr3:uid="{64031A45-824B-4700-8A01-8F0F87C05385}" name="Req. ID" dataDxfId="30"/>
@@ -3102,8 +3087,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7551B106-1BC4-4794-8DF3-1BDFDAFF6E5D}">
   <dimension ref="A1:V321"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3145,11 +3130,11 @@
       <c r="P1" s="4"/>
       <c r="Q1" s="5"/>
       <c r="R1" s="4"/>
-      <c r="T1" s="21" t="s">
+      <c r="T1" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="U1" s="21"/>
-      <c r="V1" s="21"/>
+      <c r="U1" s="20"/>
+      <c r="V1" s="20"/>
     </row>
     <row r="2" spans="1:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
@@ -3170,11 +3155,11 @@
       <c r="P2" s="4"/>
       <c r="Q2" s="5"/>
       <c r="R2" s="4"/>
-      <c r="T2" s="22" t="s">
+      <c r="T2" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="U2" s="22"/>
-      <c r="V2" s="22"/>
+      <c r="U2" s="21"/>
+      <c r="V2" s="21"/>
     </row>
     <row r="3" spans="1:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
@@ -3183,57 +3168,57 @@
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
-      <c r="G3" s="31" t="s">
+      <c r="G3" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="H3" s="31"/>
-      <c r="I3" s="31"/>
-      <c r="J3" s="31"/>
-      <c r="K3" s="31"/>
-      <c r="L3" s="31"/>
-      <c r="M3" s="31"/>
-      <c r="N3" s="31"/>
-      <c r="O3" s="31"/>
+      <c r="H3" s="30"/>
+      <c r="I3" s="30"/>
+      <c r="J3" s="30"/>
+      <c r="K3" s="30"/>
+      <c r="L3" s="30"/>
+      <c r="M3" s="30"/>
+      <c r="N3" s="30"/>
+      <c r="O3" s="30"/>
       <c r="P3" s="4"/>
       <c r="Q3" s="5"/>
       <c r="R3" s="4"/>
-      <c r="T3" s="22" t="s">
+      <c r="T3" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="U3" s="22"/>
-      <c r="V3" s="22"/>
+      <c r="U3" s="21"/>
+      <c r="V3" s="21"/>
     </row>
     <row r="4" spans="1:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="28" t="s">
+      <c r="A4" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="28"/>
-      <c r="C4" s="29" t="s">
+      <c r="B4" s="27"/>
+      <c r="C4" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="D4" s="30"/>
+      <c r="D4" s="29"/>
       <c r="E4" s="19"/>
       <c r="F4" s="4"/>
-      <c r="G4" s="31"/>
-      <c r="H4" s="31"/>
-      <c r="I4" s="31"/>
-      <c r="J4" s="31"/>
-      <c r="K4" s="31"/>
-      <c r="L4" s="31"/>
-      <c r="M4" s="31"/>
-      <c r="N4" s="31"/>
-      <c r="O4" s="31"/>
+      <c r="G4" s="30"/>
+      <c r="H4" s="30"/>
+      <c r="I4" s="30"/>
+      <c r="J4" s="30"/>
+      <c r="K4" s="30"/>
+      <c r="L4" s="30"/>
+      <c r="M4" s="30"/>
+      <c r="N4" s="30"/>
+      <c r="O4" s="30"/>
       <c r="P4" s="4"/>
       <c r="Q4" s="5"/>
       <c r="R4" s="4"/>
     </row>
     <row r="5" spans="1:22" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="27" t="s">
+      <c r="A5" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="27"/>
-      <c r="C5" s="29"/>
-      <c r="D5" s="30"/>
+      <c r="B5" s="26"/>
+      <c r="C5" s="28"/>
+      <c r="D5" s="29"/>
       <c r="E5" s="19"/>
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
@@ -3250,29 +3235,29 @@
       <c r="R5" s="4"/>
     </row>
     <row r="6" spans="1:22" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="23" t="s">
+      <c r="A6" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="24"/>
-      <c r="C6" s="25"/>
-      <c r="D6" s="25"/>
-      <c r="E6" s="25"/>
-      <c r="F6" s="26"/>
-      <c r="G6" s="23" t="s">
+      <c r="B6" s="23"/>
+      <c r="C6" s="24"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="25"/>
+      <c r="G6" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="H6" s="24"/>
-      <c r="I6" s="24"/>
-      <c r="J6" s="24"/>
-      <c r="K6" s="24"/>
-      <c r="L6" s="24"/>
-      <c r="M6" s="24"/>
-      <c r="N6" s="26"/>
-      <c r="O6" s="23" t="s">
+      <c r="H6" s="23"/>
+      <c r="I6" s="23"/>
+      <c r="J6" s="23"/>
+      <c r="K6" s="23"/>
+      <c r="L6" s="23"/>
+      <c r="M6" s="23"/>
+      <c r="N6" s="25"/>
+      <c r="O6" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="P6" s="24"/>
-      <c r="Q6" s="26"/>
+      <c r="P6" s="23"/>
+      <c r="Q6" s="25"/>
       <c r="R6" s="3"/>
     </row>
     <row r="7" spans="1:22" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
@@ -3334,18 +3319,16 @@
         <v>12</v>
       </c>
       <c r="T7" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A8" s="9">
-        <v>1</v>
-      </c>
-      <c r="B8" s="20" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="9"/>
+      <c r="B8" s="34" t="s">
+        <v>58</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>59</v>
-      </c>
-      <c r="C8" s="36" t="s">
-        <v>70</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="10">
@@ -3369,23 +3352,21 @@
       <c r="S8" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="T8" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A9" s="12">
-        <v>2</v>
-      </c>
-      <c r="B9" t="s">
-        <v>39</v>
+      <c r="T8" s="31" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="12"/>
+      <c r="B9" s="35" t="s">
+        <v>60</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="D9" s="1"/>
+        <v>62</v>
+      </c>
+      <c r="D9" s="31"/>
       <c r="E9" s="10">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>29</v>
@@ -3404,19 +3385,17 @@
       <c r="S9" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="T9" s="1" t="s">
-        <v>51</v>
+      <c r="T9" s="31" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A10" s="9">
-        <v>3</v>
-      </c>
-      <c r="B10" t="s">
-        <v>37</v>
+      <c r="A10" s="9"/>
+      <c r="B10" s="35" t="s">
+        <v>46</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1">
@@ -3439,23 +3418,21 @@
       <c r="S10" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="T10" s="1" t="s">
+      <c r="T10" s="31" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A11" s="12">
-        <v>4</v>
-      </c>
-      <c r="B11" t="s">
-        <v>35</v>
+      <c r="A11" s="12"/>
+      <c r="B11" s="35" t="s">
+        <v>44</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>29</v>
@@ -3474,23 +3451,21 @@
       <c r="S11" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="T11" s="1" t="s">
-        <v>51</v>
+      <c r="T11" s="31" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A12" s="9">
-        <v>5</v>
-      </c>
-      <c r="B12" t="s">
-        <v>78</v>
-      </c>
-      <c r="C12" s="10" t="s">
-        <v>97</v>
+      <c r="A12" s="9"/>
+      <c r="B12" s="35" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" s="38" t="s">
+        <v>66</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>29</v>
@@ -3509,59 +3484,58 @@
       <c r="S12" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="T12" s="1" t="s">
-        <v>52</v>
+      <c r="T12" s="31" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A13" s="12">
-        <v>6</v>
-      </c>
+      <c r="A13" s="12"/>
       <c r="B13" s="35" t="s">
-        <v>33</v>
-      </c>
-      <c r="C13" s="34" t="s">
-        <v>68</v>
+        <v>47</v>
+      </c>
+      <c r="C13" s="38" t="s">
+        <v>66</v>
       </c>
       <c r="D13" s="1"/>
-      <c r="E13" s="36">
-        <v>1</v>
-      </c>
-      <c r="F13" s="36" t="s">
+      <c r="E13" s="1">
+        <v>4</v>
+      </c>
+      <c r="F13" s="1" t="s">
         <v>29</v>
       </c>
       <c r="G13" s="13"/>
       <c r="H13" s="12"/>
-      <c r="I13" s="36"/>
-      <c r="J13" s="36"/>
-      <c r="K13" s="36"/>
-      <c r="L13" s="36"/>
-      <c r="M13" s="36"/>
-      <c r="N13" s="36"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
       <c r="O13" s="13"/>
       <c r="P13" s="12"/>
-      <c r="Q13" s="36"/>
       <c r="R13" s="13"/>
       <c r="S13" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="T13" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A14" s="9">
-        <v>7</v>
-      </c>
-      <c r="B14" t="s">
-        <v>34</v>
-      </c>
-      <c r="C14" s="36" t="s">
-        <v>72</v>
+      <c r="T13" s="31" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="9"/>
+      <c r="B14" s="35" t="s">
+        <v>49</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
+      <c r="E14" s="1">
+        <v>5</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="G14" s="13"/>
       <c r="H14" s="12"/>
       <c r="I14" s="1"/>
@@ -3573,22 +3547,24 @@
       <c r="O14" s="13"/>
       <c r="P14" s="12"/>
       <c r="R14" s="13"/>
-      <c r="S14" s="17"/>
-      <c r="T14" s="1"/>
-    </row>
-    <row r="15" spans="1:22" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="12">
-        <v>8</v>
-      </c>
-      <c r="B15" t="s">
-        <v>73</v>
+      <c r="S14" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="T14" s="31" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A15" s="12"/>
+      <c r="B15" s="35" t="s">
+        <v>45</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="D15" s="1"/>
-      <c r="E15" s="1">
-        <v>3</v>
+      <c r="E15" s="32">
+        <v>10</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>29</v>
@@ -3607,23 +3583,21 @@
       <c r="S15" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="T15" s="1" t="s">
-        <v>54</v>
+      <c r="T15" s="31" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A16" s="12">
-        <v>9</v>
-      </c>
-      <c r="B16" t="s">
-        <v>36</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>71</v>
+      <c r="A16" s="12"/>
+      <c r="B16" s="35" t="s">
+        <v>50</v>
+      </c>
+      <c r="C16" s="32" t="s">
+        <v>74</v>
       </c>
       <c r="D16" s="1"/>
       <c r="E16" s="1">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>29</v>
@@ -3642,19 +3616,17 @@
       <c r="S16" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="T16" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A17" s="9">
-        <v>10</v>
-      </c>
-      <c r="B17" t="s">
-        <v>43</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>77</v>
+      <c r="T16" s="31" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="9"/>
+      <c r="B17" s="36" t="s">
+        <v>37</v>
+      </c>
+      <c r="C17" s="32" t="s">
+        <v>69</v>
       </c>
       <c r="D17" s="1"/>
       <c r="E17" s="1">
@@ -3677,22 +3649,20 @@
       <c r="S17" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="T17" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="18" spans="1:20" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="12">
-        <v>11</v>
-      </c>
-      <c r="B18" t="s">
-        <v>42</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>76</v>
+      <c r="T17" s="31" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A18" s="12"/>
+      <c r="B18" s="36" t="s">
+        <v>61</v>
+      </c>
+      <c r="C18" s="31" t="s">
+        <v>73</v>
       </c>
       <c r="D18" s="1"/>
-      <c r="E18" s="1">
+      <c r="E18" s="32">
         <v>1</v>
       </c>
       <c r="F18" s="1" t="s">
@@ -3712,23 +3682,21 @@
       <c r="S18" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="T18" s="1" t="s">
-        <v>52</v>
+      <c r="T18" s="31" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A19" s="12">
-        <v>12</v>
-      </c>
-      <c r="B19" t="s">
-        <v>38</v>
+      <c r="A19" s="12"/>
+      <c r="B19" s="36" t="s">
+        <v>35</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>98</v>
+        <v>70</v>
       </c>
       <c r="D19" s="1"/>
       <c r="E19" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>29</v>
@@ -3747,23 +3715,21 @@
       <c r="S19" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="T19" s="1" t="s">
-        <v>52</v>
+      <c r="T19" s="31" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A20" s="12">
-        <v>13</v>
-      </c>
-      <c r="B20" t="s">
-        <v>41</v>
+      <c r="A20" s="12"/>
+      <c r="B20" s="35" t="s">
+        <v>39</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>99</v>
+        <v>72</v>
       </c>
       <c r="D20" s="1"/>
       <c r="E20" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>29</v>
@@ -3782,58 +3748,55 @@
       <c r="S20" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="T20" s="1" t="s">
-        <v>52</v>
+      <c r="T20" s="31" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A21" s="12">
-        <v>14</v>
-      </c>
-      <c r="B21" t="s">
-        <v>45</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1">
-        <v>10</v>
-      </c>
-      <c r="F21" s="1" t="s">
+      <c r="A21" s="12"/>
+      <c r="B21" s="37" t="s">
+        <v>33</v>
+      </c>
+      <c r="C21" s="33" t="s">
+        <v>71</v>
+      </c>
+      <c r="D21" s="32"/>
+      <c r="E21" s="32">
+        <v>1</v>
+      </c>
+      <c r="F21" s="32" t="s">
         <v>29</v>
       </c>
       <c r="G21" s="13"/>
       <c r="H21" s="12"/>
-      <c r="I21" s="1"/>
-      <c r="J21" s="1"/>
-      <c r="K21" s="1"/>
-      <c r="L21" s="1"/>
-      <c r="M21" s="1"/>
-      <c r="N21" s="1"/>
+      <c r="I21" s="32"/>
+      <c r="J21" s="32"/>
+      <c r="K21" s="32"/>
+      <c r="L21" s="32"/>
+      <c r="M21" s="32"/>
+      <c r="N21" s="32"/>
       <c r="O21" s="13"/>
       <c r="P21" s="12"/>
+      <c r="Q21" s="32"/>
       <c r="R21" s="13"/>
       <c r="S21" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="T21" s="1" t="s">
-        <v>53</v>
+      <c r="T21" s="31" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A22" s="12">
-        <v>15</v>
-      </c>
-      <c r="B22" t="s">
-        <v>100</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>101</v>
+      <c r="A22" s="12"/>
+      <c r="B22" s="36" t="s">
+        <v>36</v>
+      </c>
+      <c r="C22" s="32" t="s">
+        <v>75</v>
       </c>
       <c r="D22" s="1"/>
-      <c r="E22" s="36">
-        <v>10</v>
+      <c r="E22" s="1">
+        <v>3</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>29</v>
@@ -3852,55 +3815,43 @@
       <c r="S22" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="T22" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="23" spans="1:20" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="12">
-        <v>16</v>
-      </c>
-      <c r="B23" s="35" t="s">
+      <c r="T22" s="31" t="s">
         <v>56</v>
       </c>
-      <c r="C23" s="36" t="s">
-        <v>57</v>
-      </c>
-      <c r="D23" s="1"/>
-      <c r="E23" s="36">
-        <v>1</v>
-      </c>
-      <c r="F23" s="36" t="s">
-        <v>29</v>
-      </c>
-      <c r="G23" s="13"/>
-      <c r="H23" s="12"/>
-      <c r="I23" s="36"/>
-      <c r="J23" s="36"/>
-      <c r="K23" s="36"/>
-      <c r="L23" s="36"/>
-      <c r="M23" s="36"/>
-      <c r="N23" s="36"/>
-      <c r="O23" s="13"/>
-      <c r="P23" s="12"/>
-      <c r="Q23" s="36"/>
-      <c r="R23" s="13"/>
-      <c r="S23" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="T23" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A24" s="12">
-        <v>17</v>
-      </c>
-      <c r="B24" t="s">
-        <v>48</v>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A23" s="39"/>
+      <c r="B23" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D23" s="31"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="31"/>
+      <c r="G23" s="40"/>
+      <c r="H23" s="39"/>
+      <c r="I23" s="31"/>
+      <c r="J23" s="31"/>
+      <c r="K23" s="31"/>
+      <c r="L23" s="31"/>
+      <c r="M23" s="31"/>
+      <c r="N23" s="31"/>
+      <c r="O23" s="40"/>
+      <c r="P23" s="39"/>
+      <c r="Q23" s="31"/>
+      <c r="R23" s="40"/>
+      <c r="S23" s="41"/>
+      <c r="T23" s="31"/>
+    </row>
+    <row r="24" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="12"/>
+      <c r="B24" s="36" t="s">
+        <v>77</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D24" s="1"/>
       <c r="E24" s="1">
@@ -3923,58 +3874,55 @@
       <c r="S24" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="T24" s="1" t="s">
-        <v>52</v>
+      <c r="T24" s="31" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A25" s="12">
-        <v>18</v>
-      </c>
-      <c r="B25" t="s">
-        <v>95</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1">
-        <v>1</v>
+      <c r="A25" s="12"/>
+      <c r="B25" s="37" t="s">
+        <v>32</v>
+      </c>
+      <c r="C25" s="32" t="s">
+        <v>79</v>
+      </c>
+      <c r="D25" s="32"/>
+      <c r="E25" s="32">
+        <v>10</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>29</v>
       </c>
       <c r="G25" s="13"/>
       <c r="H25" s="12"/>
-      <c r="I25" s="1"/>
-      <c r="J25" s="1"/>
-      <c r="K25" s="1"/>
-      <c r="L25" s="1"/>
-      <c r="M25" s="1"/>
-      <c r="N25" s="1"/>
+      <c r="I25" s="32"/>
+      <c r="J25" s="32"/>
+      <c r="K25" s="32"/>
+      <c r="L25" s="32"/>
+      <c r="M25" s="32"/>
+      <c r="N25" s="32"/>
       <c r="O25" s="13"/>
       <c r="P25" s="12"/>
+      <c r="Q25" s="32"/>
       <c r="R25" s="13"/>
       <c r="S25" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="T25" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A26" s="12">
-        <v>19</v>
-      </c>
-      <c r="B26" s="32" t="s">
-        <v>32</v>
-      </c>
-      <c r="C26" s="37" t="s">
-        <v>75</v>
+      <c r="T25" s="31" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="12"/>
+      <c r="B26" s="35" t="s">
+        <v>42</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>80</v>
       </c>
       <c r="D26" s="1"/>
       <c r="E26" s="1">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>29</v>
@@ -3993,19 +3941,17 @@
       <c r="S26" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="T26" s="1" t="s">
+      <c r="T26" s="31" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A27" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="B27" t="s">
-        <v>46</v>
-      </c>
-      <c r="C27" s="36" t="s">
-        <v>61</v>
+      <c r="A27" s="12"/>
+      <c r="B27" s="35" t="s">
+        <v>43</v>
+      </c>
+      <c r="C27" s="32" t="s">
+        <v>81</v>
       </c>
       <c r="D27" s="1"/>
       <c r="E27" s="1">
@@ -4028,23 +3974,21 @@
       <c r="S27" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="T27" s="1" t="s">
-        <v>53</v>
+      <c r="T27" s="31" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A28" s="12" t="s">
-        <v>105</v>
-      </c>
-      <c r="B28" t="s">
-        <v>44</v>
+      <c r="A28" s="12"/>
+      <c r="B28" s="35" t="s">
+        <v>51</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>62</v>
+        <v>82</v>
       </c>
       <c r="D28" s="1"/>
       <c r="E28" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F28" s="1" t="s">
         <v>29</v>
@@ -4063,23 +4007,21 @@
       <c r="S28" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="T28" s="1" t="s">
-        <v>53</v>
+      <c r="T28" s="31" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A29" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="B29" t="s">
-        <v>47</v>
-      </c>
-      <c r="C29" s="33" t="s">
-        <v>94</v>
+      <c r="A29" s="12"/>
+      <c r="B29" s="35" t="s">
+        <v>83</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>84</v>
       </c>
       <c r="D29" s="1"/>
       <c r="E29" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F29" s="1" t="s">
         <v>29</v>
@@ -4098,19 +4040,17 @@
       <c r="S29" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="T29" s="1" t="s">
-        <v>53</v>
+      <c r="T29" s="31" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A30" s="12" t="s">
-        <v>106</v>
-      </c>
-      <c r="B30" t="s">
-        <v>40</v>
-      </c>
-      <c r="C30" s="33" t="s">
-        <v>93</v>
+      <c r="A30" s="12"/>
+      <c r="B30" s="35" t="s">
+        <v>48</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>85</v>
       </c>
       <c r="D30" s="1"/>
       <c r="E30" s="1">
@@ -4133,23 +4073,19 @@
       <c r="S30" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="T30" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="31" spans="1:20" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="12" t="s">
-        <v>104</v>
-      </c>
-      <c r="B31" t="s">
-        <v>58</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>60</v>
-      </c>
+      <c r="T30" s="31" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A31" s="12"/>
+      <c r="B31" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="C31" s="1"/>
       <c r="D31" s="1"/>
-      <c r="E31" s="36">
-        <v>1</v>
+      <c r="E31" s="1">
+        <v>5</v>
       </c>
       <c r="F31" s="1" t="s">
         <v>29</v>
@@ -4168,20 +4104,16 @@
       <c r="S31" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="T31" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="32" spans="1:20" ht="30" x14ac:dyDescent="0.25">
-      <c r="A32" s="12" t="s">
-        <v>107</v>
-      </c>
-      <c r="B32" t="s">
-        <v>49</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>64</v>
-      </c>
+      <c r="T31" s="31" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A32" s="12"/>
+      <c r="B32" s="35" t="s">
+        <v>38</v>
+      </c>
+      <c r="C32" s="32"/>
       <c r="D32" s="1"/>
       <c r="E32" s="1">
         <v>5</v>
@@ -4203,13 +4135,13 @@
       <c r="S32" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="T32" s="1" t="s">
-        <v>53</v>
+      <c r="T32" s="31" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="33" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A33" s="12"/>
-      <c r="B33" s="1"/>
+      <c r="B33" s="31"/>
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
@@ -4228,7 +4160,7 @@
       <c r="S33" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="T33" s="1"/>
+      <c r="T33" s="31"/>
     </row>
     <row r="34" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
@@ -4271,7 +4203,7 @@
     <row r="36" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="1" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
@@ -4292,7 +4224,7 @@
     <row r="37" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" s="1" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
@@ -4313,10 +4245,10 @@
     <row r="38" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="1" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
@@ -4336,7 +4268,7 @@
     <row r="39" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="B39" s="1" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
@@ -4357,10 +4289,10 @@
     <row r="40" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="B40" s="1" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="D40" s="1"/>
       <c r="E40" s="1"/>
@@ -4380,10 +4312,10 @@
     <row r="41" spans="1:20" ht="45" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="B41" s="1" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="D41" s="1"/>
       <c r="E41" s="1"/>
@@ -4403,10 +4335,10 @@
     <row r="42" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
       <c r="B42" s="1" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="D42" s="1"/>
       <c r="E42" s="1"/>
@@ -4426,10 +4358,10 @@
     <row r="43" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
       <c r="B43" s="1" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D43" s="1"/>
       <c r="E43" s="1"/>
@@ -4449,7 +4381,7 @@
     <row r="44" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
       <c r="B44" s="1" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="C44" s="1"/>
       <c r="D44" s="1"/>
@@ -4470,7 +4402,7 @@
     <row r="45" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
       <c r="B45" s="1" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>

</xml_diff>